<commit_message>
IN-940 Set a fixed start date for all fee reductions (01/04/2021) and a default end date for edge cases
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Fee_Reductions.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Fee_Reductions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A7087-0221-D74A-AB36-EBA512008315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2416EFEE-D6DD-D84A-9772-89EF8CE05716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="5100" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
   <si>
     <t>table_name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Award Date</t>
   </si>
   <si>
-    <t>fee_reduction_start_date</t>
-  </si>
-  <si>
     <t>EXEMPTION</t>
   </si>
   <si>
@@ -192,12 +189,15 @@
     <t>clients</t>
   </si>
   <si>
+    <t>2021-04-01</t>
+  </si>
+  <si>
     <t>exclude_values = {"col": "Remis", "values": ["0"]}
-date_since = {"col": "Award Date", "date": "31/03/2021"}</t>
+date_since = {"col": "Award Date", "date": "02/04/2021"}</t>
   </si>
   <si>
     <t>exclude_values = {"col": "Exempt", "values": ["0"]}
-date_since = {"col": "Award Date", "date": "31/03/2021"}</t>
+date_since = {"col": "Award Date", "date": "02/04/2021"}</t>
   </si>
 </sst>
 </file>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -285,6 +285,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D765A69-DF19-B84F-A530-22008AF977F3}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -547,10 +553,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>31</v>
@@ -565,7 +571,7 @@
         <v>56</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.15">
@@ -573,10 +579,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>31</v>
@@ -591,7 +597,7 @@
         <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -606,9 +612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O948"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -624,7 +630,7 @@
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="32.6640625" customWidth="1"/>
@@ -664,7 +670,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -699,7 +705,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
@@ -725,7 +731,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
         <v>17</v>
@@ -754,7 +760,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="M4" s="3"/>
@@ -782,7 +788,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="3"/>
       <c r="N5" s="4" t="s">
         <v>29</v>
@@ -806,18 +812,14 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="4" t="s">
         <v>17</v>
@@ -849,7 +851,7 @@
         <v>48</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="3"/>
       <c r="N7" s="8" t="s">
         <v>17</v>
@@ -875,7 +877,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="M8" s="3"/>
@@ -903,7 +905,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3" t="b">
+      <c r="L9" s="10" t="b">
         <v>0</v>
       </c>
       <c r="M9" s="3"/>
@@ -924,7 +926,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -940,7 +942,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
@@ -956,7 +958,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
@@ -972,7 +974,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
@@ -988,7 +990,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
@@ -1004,7 +1006,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
@@ -1798,9 +1800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B535CC52-A970-3842-B87A-7B605287A215}">
   <dimension ref="A1:O948"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1816,7 +1818,7 @@
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="32.6640625" customWidth="1"/>
@@ -1856,7 +1858,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1891,7 +1893,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
@@ -1917,7 +1919,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
         <v>17</v>
@@ -1946,8 +1948,8 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="4" t="s">
-        <v>51</v>
+      <c r="L4" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
@@ -1974,7 +1976,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="3"/>
       <c r="N5" s="4" t="s">
         <v>29</v>
@@ -1998,18 +2000,14 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="4" t="s">
         <v>17</v>
@@ -2041,7 +2039,7 @@
         <v>48</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="3"/>
       <c r="N7" s="8" t="s">
         <v>17</v>
@@ -2067,7 +2065,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="M8" s="3"/>
@@ -2095,7 +2093,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3" t="b">
+      <c r="L9" s="10" t="b">
         <v>0</v>
       </c>
       <c r="M9" s="3"/>
@@ -2116,7 +2114,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -2132,7 +2130,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
@@ -2148,7 +2146,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
@@ -2164,7 +2162,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
@@ -2180,7 +2178,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
@@ -2196,7 +2194,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>

</xml_diff>

<commit_message>
IN-940 Tweaks to fee reduction mapping and transformations (#423)
* IN-940 Set a fixed start date for all fee reductions (01/04/2021) and a default end date for edge cases

* Fix bond_providers in pre
</commit_message>
<xml_diff>
--- a/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Fee_Reductions.xlsx
+++ b/migration_steps/shared/mapping_spreadsheet/Casrec_Mapping_Document_Fee_Reductions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration-mappings/mapping_spreadsheet/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dimitarkokov/PycharmProjects/opg-data-casrec-migration/migration_steps/shared/mapping_spreadsheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B81A7087-0221-D74A-AB36-EBA512008315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2416EFEE-D6DD-D84A-9772-89EF8CE05716}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2580" yWindow="5100" windowWidth="33600" windowHeight="20540" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="table_definitions" sheetId="4" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="58">
   <si>
     <t>table_name</t>
   </si>
@@ -174,9 +174,6 @@
     <t>Award Date</t>
   </si>
   <si>
-    <t>fee_reduction_start_date</t>
-  </si>
-  <si>
     <t>EXEMPTION</t>
   </si>
   <si>
@@ -192,12 +189,15 @@
     <t>clients</t>
   </si>
   <si>
+    <t>2021-04-01</t>
+  </si>
+  <si>
     <t>exclude_values = {"col": "Remis", "values": ["0"]}
-date_since = {"col": "Award Date", "date": "31/03/2021"}</t>
+date_since = {"col": "Award Date", "date": "02/04/2021"}</t>
   </si>
   <si>
     <t>exclude_values = {"col": "Exempt", "values": ["0"]}
-date_since = {"col": "Award Date", "date": "31/03/2021"}</t>
+date_since = {"col": "Award Date", "date": "02/04/2021"}</t>
   </si>
 </sst>
 </file>
@@ -271,7 +271,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -285,6 +285,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D765A69-DF19-B84F-A530-22008AF977F3}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -547,10 +553,10 @@
         <v>41</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>31</v>
@@ -565,7 +571,7 @@
         <v>56</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="56" x14ac:dyDescent="0.15">
@@ -573,10 +579,10 @@
         <v>42</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>31</v>
@@ -591,7 +597,7 @@
         <v>57</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.15">
@@ -606,9 +612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O948"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomLeft" activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -624,7 +630,7 @@
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="32.6640625" customWidth="1"/>
@@ -664,7 +670,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -699,7 +705,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
@@ -725,7 +731,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
         <v>17</v>
@@ -754,7 +760,7 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="3" t="s">
+      <c r="L4" s="10" t="s">
         <v>44</v>
       </c>
       <c r="M4" s="3"/>
@@ -782,7 +788,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="3"/>
       <c r="N5" s="4" t="s">
         <v>29</v>
@@ -806,18 +812,14 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="4" t="s">
         <v>17</v>
@@ -849,7 +851,7 @@
         <v>48</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="3"/>
       <c r="N7" s="8" t="s">
         <v>17</v>
@@ -875,7 +877,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="M8" s="3"/>
@@ -903,7 +905,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3" t="b">
+      <c r="L9" s="10" t="b">
         <v>0</v>
       </c>
       <c r="M9" s="3"/>
@@ -924,7 +926,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -940,7 +942,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
@@ -956,7 +958,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
@@ -972,7 +974,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
@@ -988,7 +990,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
@@ -1004,7 +1006,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>
@@ -1798,9 +1800,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B535CC52-A970-3842-B87A-7B605287A215}">
   <dimension ref="A1:O948"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1816,7 +1818,7 @@
     <col min="9" max="9" width="20" customWidth="1"/>
     <col min="10" max="10" width="23.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="21.33203125" customWidth="1"/>
-    <col min="12" max="12" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.83203125" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="11.5" customWidth="1"/>
     <col min="14" max="14" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="32.6640625" customWidth="1"/>
@@ -1856,7 +1858,7 @@
       <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="L1" s="9" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1891,7 +1893,7 @@
       <c r="I2" s="3"/>
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
-      <c r="L2" s="3"/>
+      <c r="L2" s="10"/>
       <c r="M2" s="3"/>
       <c r="N2" s="3"/>
     </row>
@@ -1917,7 +1919,7 @@
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
+      <c r="L3" s="10"/>
       <c r="M3" s="3"/>
       <c r="N3" s="4" t="s">
         <v>17</v>
@@ -1946,8 +1948,8 @@
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
       <c r="K4" s="3"/>
-      <c r="L4" s="4" t="s">
-        <v>51</v>
+      <c r="L4" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3" t="s">
@@ -1974,7 +1976,7 @@
       <c r="I5" s="3"/>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
+      <c r="L5" s="10"/>
       <c r="M5" s="3"/>
       <c r="N5" s="4" t="s">
         <v>29</v>
@@ -1998,18 +2000,14 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
-      <c r="G6" s="4" t="s">
-        <v>43</v>
-      </c>
+      <c r="G6" s="4"/>
       <c r="H6" s="3"/>
-      <c r="I6" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>50</v>
-      </c>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
       <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
+      <c r="L6" s="10" t="s">
+        <v>55</v>
+      </c>
       <c r="M6" s="3"/>
       <c r="N6" s="4" t="s">
         <v>17</v>
@@ -2041,7 +2039,7 @@
         <v>48</v>
       </c>
       <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
+      <c r="L7" s="10"/>
       <c r="M7" s="3"/>
       <c r="N7" s="8" t="s">
         <v>17</v>
@@ -2067,7 +2065,7 @@
       <c r="I8" s="3"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="11" t="s">
         <v>45</v>
       </c>
       <c r="M8" s="3"/>
@@ -2095,7 +2093,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
       <c r="K9" s="3"/>
-      <c r="L9" s="3" t="b">
+      <c r="L9" s="10" t="b">
         <v>0</v>
       </c>
       <c r="M9" s="3"/>
@@ -2116,7 +2114,7 @@
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
       <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
     </row>
@@ -2132,7 +2130,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
+      <c r="L11" s="10"/>
       <c r="M11" s="3"/>
       <c r="N11" s="3"/>
     </row>
@@ -2148,7 +2146,7 @@
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
+      <c r="L12" s="10"/>
       <c r="M12" s="3"/>
       <c r="N12" s="3"/>
     </row>
@@ -2164,7 +2162,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
+      <c r="L13" s="10"/>
       <c r="M13" s="3"/>
       <c r="N13" s="3"/>
     </row>
@@ -2180,7 +2178,7 @@
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
+      <c r="L14" s="10"/>
       <c r="M14" s="3"/>
       <c r="N14" s="3"/>
     </row>
@@ -2196,7 +2194,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
+      <c r="L15" s="10"/>
       <c r="M15" s="3"/>
       <c r="N15" s="3"/>
     </row>

</xml_diff>